<commit_message>
Add some formatting to fixture in the middle of a cell
This is in order to test this change for .ods:
https://github.com/OpenDataServices/flatten-tool/commit/3c37290fa077cdea39c3a7d09689fe7118b7a056
</commit_message>
<xml_diff>
--- a/flattentool/tests/fixtures/xlsx/basic.xlsx
+++ b/flattentool/tests/fixtures/xlsx/basic.xlsx
@@ -5,53 +5,85 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="319" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="subsheet" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>colA</t>
-  </si>
-  <si>
-    <t>colB</t>
-  </si>
-  <si>
-    <t>cell1</t>
-  </si>
-  <si>
-    <t>cell2</t>
-  </si>
-  <si>
-    <t>cell3</t>
-  </si>
-  <si>
-    <t>cell4</t>
-  </si>
-  <si>
-    <t>colC</t>
-  </si>
-  <si>
-    <t>colD</t>
-  </si>
-  <si>
-    <t>cell5</t>
-  </si>
-  <si>
-    <t>cell6</t>
-  </si>
-  <si>
-    <t>cell7</t>
-  </si>
-  <si>
-    <t>cell8</t>
+    <t xml:space="preserve">colA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colD</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ce</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ll</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">5</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">cell6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell8</t>
   </si>
 </sst>
 </file>
@@ -59,9 +91,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -82,6 +114,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,13 +190,13 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -187,7 +226,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -203,13 +242,13 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,7 +278,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>